<commit_message>
update multiple stat files
</commit_message>
<xml_diff>
--- a/NFLStats/CB/CB_aggregate.xlsx
+++ b/NFLStats/CB/CB_aggregate.xlsx
@@ -33,7 +33,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -44,6 +44,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00CCFFCC"/>
         <bgColor rgb="00CCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFBD"/>
+        <bgColor rgb="00FFFFBD"/>
       </patternFill>
     </fill>
   </fills>
@@ -74,12 +80,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,6 +564,150 @@
         <v>8.666666666666668</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Denzel Ward</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>44.33333333333334</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>36.66666666666666</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>7.666666666666667</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Denzel Ward</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>45.33333333333334</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>37.66666666666666</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>7.666666666666667</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>Denzel Ward</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Isaac Yiadom</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>23.33333333333333</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>9.666666666666666</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Isaac Yiadom</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>28.11111111111111</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>21.22222222222222</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>6.888888888888888</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Isaac Yiadom</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>3.666666666666667</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>-4.888888888888886</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>-2.111111111111107</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>-2.777777777777778</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ran player stats and deleted non compatible
</commit_message>
<xml_diff>
--- a/NFLStats/CB/CB_aggregate.xlsx
+++ b/NFLStats/CB/CB_aggregate.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -708,6 +708,222 @@
         <v>-2.777777777777778</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>Charvarius Ward</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>8.666666666666666</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>47.33333333333334</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>16.66666666666667</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>Charvarius Ward</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>13.66666666666667</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>51</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>Charvarius Ward</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>3.666666666666664</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>3.333333333333332</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>J.T. Gray</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>15.66666666666667</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>2.666666666666667</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>J.T. Gray</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>9.333333333333334</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>8.666666666666666</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>J.T. Gray</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>-0.3333333333333333</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>2.333333333333334</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>-3.666666666666666</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>Mike Ford</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>8.666666666666666</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>1.333333333333333</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>Mike Ford</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>18.66666666666667</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>13.33333333333333</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>Mike Ford</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>-0.3333333333333334</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>8.666666666666668</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>4.666666666666668</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>